<commit_message>
productDetailPage- selecting product with and without variants
</commit_message>
<xml_diff>
--- a/src/com/styletag/test_cases/TestSuit.xlsx
+++ b/src/com/styletag/test_cases/TestSuit.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="17">
   <si>
     <t xml:space="preserve">Test Scenario</t>
   </si>
@@ -68,6 +68,9 @@
   </si>
   <si>
     <t xml:space="preserve">“3”</t>
+  </si>
+  <si>
+    <t xml:space="preserve">productDetailPage</t>
   </si>
 </sst>
 </file>
@@ -77,7 +80,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -112,12 +115,6 @@
       <name val="Monospace"/>
       <family val="0"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Monospace"/>
-      <family val="0"/>
     </font>
   </fonts>
   <fills count="2">
@@ -162,7 +159,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -176,10 +173,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -203,17 +196,17 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D3" activeCellId="0" sqref="D3"/>
+      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.4387755102041"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.280612244898"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="17.5510204081633"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="25.1071428571429"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="14.4438775510204"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.8979591836735"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.7397959183673"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="17.0102040816327"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="24.5663265306122"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="13.9030612244898"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -263,7 +256,7 @@
       <c r="D3" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="E3" s="4"/>
+      <c r="E3" s="3"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
@@ -275,8 +268,11 @@
       <c r="C4" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="D4" s="3" t="s">
         <v>8</v>
+      </c>
+      <c r="E4" s="0" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
ExcleWrite file- included new function for writeing to desired column(format of log sheet changed)
</commit_message>
<xml_diff>
--- a/src/com/styletag/test_cases/TestSuit.xlsx
+++ b/src/com/styletag/test_cases/TestSuit.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="25">
   <si>
     <t xml:space="preserve">Test Scenario</t>
   </si>
@@ -46,31 +46,55 @@
     <t xml:space="preserve">NO</t>
   </si>
   <si>
+    <t xml:space="preserve">login</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Search Page</t>
+  </si>
+  <si>
+    <t xml:space="preserve">“2”</t>
+  </si>
+  <si>
+    <t xml:space="preserve">YES</t>
+  </si>
+  <si>
+    <t xml:space="preserve">search</t>
+  </si>
+  <si>
+    <t xml:space="preserve">applyFilters</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Product Listing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">“3”</t>
+  </si>
+  <si>
     <t xml:space="preserve">productCatalogPage</t>
   </si>
   <si>
-    <t xml:space="preserve">applyFilters</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Search</t>
-  </si>
-  <si>
-    <t xml:space="preserve">“2”</t>
-  </si>
-  <si>
-    <t xml:space="preserve">YES</t>
-  </si>
-  <si>
-    <t xml:space="preserve">search</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Product Listing</t>
-  </si>
-  <si>
-    <t xml:space="preserve">“3”</t>
-  </si>
-  <si>
     <t xml:space="preserve">productDetailPage</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Checking Filters</t>
+  </si>
+  <si>
+    <t xml:space="preserve">“4”</t>
+  </si>
+  <si>
+    <t xml:space="preserve">COD Order</t>
+  </si>
+  <si>
+    <t xml:space="preserve">“5”</t>
+  </si>
+  <si>
+    <t xml:space="preserve">clearCart</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cartCheck</t>
+  </si>
+  <si>
+    <t xml:space="preserve">checkout</t>
   </si>
 </sst>
 </file>
@@ -80,7 +104,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="9">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -108,6 +132,24 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Monospace"/>
+      <family val="1"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Monospace"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
@@ -159,7 +201,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -173,6 +215,18 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -193,7 +247,7 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
@@ -201,12 +255,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.8979591836735"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.7397959183673"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="17.0102040816327"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="24.5663265306122"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="13.9030612244898"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.3571428571429"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.2857142857143"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.7704081632653"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="23.8928571428571"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="25.5561224489796"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="25.2448979591837"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="17.8214285714286"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="12.9591836734694"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -226,7 +283,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
@@ -239,24 +296,23 @@
       <c r="D2" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="0" t="s">
-        <v>9</v>
-      </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="0" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="C3" s="0" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="0" t="s">
+      <c r="D3" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="D3" s="0" t="s">
+      <c r="E3" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="E3" s="3"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
@@ -266,13 +322,62 @@
         <v>15</v>
       </c>
       <c r="C4" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="F4" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="D4" s="3" t="s">
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E4" s="0" t="s">
+      <c r="E6" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F6" s="6" t="s">
         <v>16</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="H6" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="I6" s="0" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>